<commit_message>
add single class in each test tag
</commit_message>
<xml_diff>
--- a/test-data/XCOV19.xlsx
+++ b/test-data/XCOV19.xlsx
@@ -70,7 +70,7 @@
     <t>invalid</t>
   </si>
   <si>
-    <t>myCovidConnect13@gmail.com</t>
+    <t>myCovidConnect21@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -408,7 +408,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:B5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add logs to test files
</commit_message>
<xml_diff>
--- a/test-data/XCOV19.xlsx
+++ b/test-data/XCOV19.xlsx
@@ -70,7 +70,7 @@
     <t>invalid</t>
   </si>
   <si>
-    <t>myCovidConnect21@gmail.com</t>
+    <t>myCovidConnect25@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -470,7 +470,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>